<commit_message>
updated script sprint 1
added code to calculate infection risk + read in text files for scenarios and exposure
</commit_message>
<xml_diff>
--- a/examples/Data bronnen/Model parameters QMRA.xlsx
+++ b/examples/Data bronnen/Model parameters QMRA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/julia_bleser_deltares_nl/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harezlak\Githubprojects\FloodsandHealth\FloodsAndHealthTool\examples\Data bronnen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{5A020FCD-15DB-4FFE-AEAC-A6287ED3360C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05A1E39D-07FB-42E2-A71B-54157DE47CAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF076CD-CCB2-4E3D-9DEB-1CD0F69F5BCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DCEF2428-4976-46D2-B85B-8DDF3C37A4F6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{DCEF2428-4976-46D2-B85B-8DDF3C37A4F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="2" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -879,9 +877,6 @@
     <t>no dilution</t>
   </si>
   <si>
-    <t>P_inf= 1 - (1+ (d/N50) * 2^(1/a)-1))^-a</t>
-  </si>
-  <si>
     <t>Beta-Poisson model</t>
   </si>
   <si>
@@ -955,6 +950,9 @@
   </si>
   <si>
     <t>P_event= 1 - (1+ (d/N50) * 2^(1/a)-1))^-a</t>
+  </si>
+  <si>
+    <t>P_inf= 1 - (1+ (d/N50) * (2^(1/a)-1))^-a</t>
   </si>
 </sst>
 </file>
@@ -1158,17 +1156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1176,25 +1169,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1206,12 +1187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1221,7 +1196,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2028,21 +2026,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9A2FB2-901A-40F1-A65A-0E3F855B4A3F}">
   <dimension ref="A2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>46</v>
       </c>
@@ -2059,8 +2057,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4"/>
@@ -2068,8 +2066,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>1</v>
@@ -2090,8 +2088,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4"/>
@@ -2099,8 +2097,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>14</v>
@@ -2112,12 +2110,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -2126,9 +2124,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2141,9 +2139,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
       <c r="C13" t="s">
         <v>30</v>
       </c>
@@ -2151,9 +2149,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -2161,9 +2159,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
       <c r="C15" t="s">
         <v>32</v>
       </c>
@@ -2171,9 +2169,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" t="s">
         <v>33</v>
       </c>
@@ -2181,9 +2179,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="24"/>
+      <c r="B17" s="25"/>
       <c r="C17" t="s">
         <v>60</v>
       </c>
@@ -2197,9 +2195,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="24"/>
+      <c r="B18" s="25"/>
       <c r="C18" t="s">
         <v>56</v>
       </c>
@@ -2207,9 +2205,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="24"/>
+      <c r="B19" s="25"/>
       <c r="C19" t="s">
         <v>57</v>
       </c>
@@ -2217,12 +2215,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>34</v>
       </c>
@@ -2236,13 +2234,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2258,8 +2256,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
       <c r="B25" s="4"/>
       <c r="C25" t="s">
         <v>52</v>
@@ -2271,8 +2269,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
       <c r="B26" s="4"/>
       <c r="C26" t="s">
         <v>118</v>
@@ -2284,8 +2282,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
       <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
@@ -2299,27 +2297,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
       <c r="B29" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>303</v>
+        <v>278</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>302</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
       <c r="B30" s="4"/>
       <c r="C30" s="17" t="s">
         <v>114</v>
@@ -2329,21 +2327,21 @@
       </c>
       <c r="E30" s="17"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
       <c r="B31" s="4"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>109</v>
       </c>
@@ -2351,15 +2349,15 @@
         <v>109</v>
       </c>
       <c r="D35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
+      <c r="D36" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2383,12 +2381,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2411,7 +2409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -2454,7 +2452,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2476,7 +2474,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -2498,30 +2496,30 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6">
         <f>1.84*10^4</f>
         <v>18400</v>
       </c>
       <c r="F6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" t="s">
         <v>284</v>
       </c>
-      <c r="G6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7">
         <f>10^6</f>
@@ -2532,13 +2530,13 @@
         <v>100000000</v>
       </c>
       <c r="F7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -2560,12 +2558,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -2577,10 +2575,10 @@
         <v>119</v>
       </c>
       <c r="G9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -2617,10 +2615,10 @@
         <v>119</v>
       </c>
       <c r="G11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2676,9 +2674,9 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2713,7 +2711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -2739,7 +2737,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -2768,7 +2766,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -2788,10 +2786,10 @@
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -2811,13 +2809,13 @@
         <v>3.5</v>
       </c>
       <c r="J5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -2840,13 +2838,13 @@
         <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -2866,10 +2864,10 @@
         <v>93</v>
       </c>
       <c r="K7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -2880,7 +2878,7 @@
         <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
         <v>81</v>
@@ -2892,13 +2890,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="J8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -2909,7 +2907,7 @@
         <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
         <v>80</v>
@@ -2921,13 +2919,13 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -2961,9 +2959,9 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2983,7 +2981,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -3000,7 +2998,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -3020,10 +3018,10 @@
         <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -3043,10 +3041,10 @@
         <v>110</v>
       </c>
       <c r="H4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -3060,7 +3058,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3071,10 +3069,10 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -3088,7 +3086,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3107,15 +3105,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55861E7C-73F7-4A51-B111-5F66C724A695}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>96</v>
       </c>
@@ -3155,7 +3157,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>101</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>896</v>
       </c>
       <c r="N4">
-        <f>1-(1+J4/M4*(2^(1/K4)-1))^-K4</f>
+        <f>1-(1+(J4/M4)*(2^(1/K4)-1))^(-1*K4)</f>
         <v>7.7851098575718591E-3</v>
       </c>
       <c r="O4">
@@ -3219,7 +3221,7 @@
         <v>3.0778675501743069E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -3247,6 +3249,24 @@
       <c r="P5">
         <f>1-(1-N5)^O5</f>
         <v>0.60477911856060684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f>J4/M4</f>
+        <v>4.6874999999999998E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f>2^(1/K4)</f>
+        <v>119.14311090175811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f>(1+M9*M10-1)^(-1*K4)</f>
+        <v>1.5194398719366804</v>
       </c>
     </row>
   </sheetData>
@@ -3259,46 +3279,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC708D86-03C3-4CDD-80CD-56AA1A3539C8}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="5.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E1" s="5"/>
       <c r="F1" s="6" t="s">
         <v>135</v>
       </c>
       <c r="G1" s="6"/>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="26" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26" t="s">
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -3363,17 +3384,17 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:23" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>180</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="29" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="30" t="s">
@@ -3382,7 +3403,7 @@
       <c r="F3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="26" t="s">
         <v>185</v>
       </c>
       <c r="H3" s="12" t="s">
@@ -3419,16 +3440,16 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="33"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="12" t="s">
         <v>13</v>
       </c>
@@ -3448,16 +3469,16 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="11" t="s">
         <v>41</v>
       </c>
@@ -3484,16 +3505,16 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
       <c r="B6" s="30"/>
-      <c r="C6" s="33"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="11" t="s">
         <v>42</v>
       </c>
@@ -3520,14 +3541,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
       <c r="B7" s="30"/>
-      <c r="C7" s="33"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="11" t="s">
         <v>62</v>
       </c>
@@ -3546,14 +3567,14 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
       <c r="B8" s="30"/>
-      <c r="C8" s="33"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="28"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="11" t="s">
         <v>58</v>
       </c>
@@ -3578,14 +3599,14 @@
       </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9" s="30"/>
-      <c r="C9" s="33"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="30"/>
       <c r="E9" s="30"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="11" t="s">
         <v>148</v>
       </c>
@@ -3612,14 +3633,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="30"/>
-      <c r="C10" s="33"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="28"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="11" t="s">
         <v>48</v>
       </c>
@@ -3649,14 +3670,14 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
       <c r="B11" s="31"/>
-      <c r="C11" s="34"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="29"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="8" t="s">
         <v>63</v>
       </c>
@@ -3684,20 +3705,20 @@
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="29" t="s">
         <v>208</v>
       </c>
       <c r="F12" s="11" t="s">
@@ -3732,10 +3753,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="25"/>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
       <c r="F13" s="11" t="s">
@@ -3774,10 +3795,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="25"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="11"/>
@@ -3808,10 +3829,10 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="25"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="11"/>
@@ -3833,10 +3854,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="41"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
       <c r="F16" s="8"/>
@@ -3870,20 +3891,20 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="29" t="s">
         <v>234</v>
       </c>
       <c r="F17" s="11" t="s">
@@ -3906,8 +3927,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -3933,8 +3954,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -3955,8 +3976,8 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
       <c r="B20" s="30"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -3977,8 +3998,8 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="15"/>
@@ -4006,17 +4027,17 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="29" t="s">
         <v>250</v>
       </c>
       <c r="E22" s="16"/>
@@ -4058,10 +4079,10 @@
       </c>
       <c r="V22" s="17"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="38"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="30"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11" t="s">
@@ -4098,10 +4119,10 @@
       <c r="U23" s="19"/>
       <c r="V23" s="19"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="38"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="30"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11" t="s">
@@ -4134,10 +4155,10 @@
       <c r="U24" s="19"/>
       <c r="V24" s="19"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" s="30"/>
-      <c r="C25" s="38"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="30"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11" t="s">
@@ -4168,10 +4189,10 @@
       <c r="U25" s="19"/>
       <c r="V25" s="19"/>
     </row>
-    <row r="26" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
+    <row r="26" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="38"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="30"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11" t="s">
@@ -4204,10 +4225,10 @@
       <c r="U26" s="19"/>
       <c r="V26" s="19"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
       <c r="B27" s="31"/>
-      <c r="C27" s="39"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -4236,15 +4257,15 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A28" s="42" t="s">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
         <v>272</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>273</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>183</v>
@@ -4276,23 +4297,23 @@
       </c>
       <c r="N28" s="19"/>
       <c r="O28" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P28" s="22" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
       <c r="S28" s="19"/>
       <c r="T28" s="19"/>
       <c r="U28" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V28" s="19"/>
       <c r="W28" s="19"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A29" s="43"/>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
       <c r="B29" s="11"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4305,7 +4326,7 @@
         <v>210</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J29" s="11">
         <v>10</v>
@@ -4328,8 +4349,8 @@
       <c r="V29" s="19"/>
       <c r="W29" s="19"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A30" s="44"/>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="37"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -4363,21 +4384,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E21"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="U1:W1"/>
@@ -4387,6 +4393,21 @@
     <mergeCell ref="D3:D11"/>
     <mergeCell ref="E3:E11"/>
     <mergeCell ref="G3:G11"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4402,12 +4423,12 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -4415,7 +4436,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -4438,7 +4459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -4459,7 +4480,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -4477,7 +4498,7 @@
         <v>1700000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -4494,7 +4515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -4511,7 +4532,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -4531,7 +4552,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -4545,7 +4566,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>148</v>
       </c>
@@ -4565,7 +4586,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>48</v>
       </c>
@@ -4585,7 +4606,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>63</v>
       </c>
@@ -4602,7 +4623,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>62</v>
       </c>
@@ -4613,7 +4634,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -4634,7 +4655,7 @@
         <v>0.36399189481416838</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>165</v>
       </c>
@@ -4642,7 +4663,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>48</v>
       </c>
@@ -4653,7 +4674,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -4664,9 +4685,9 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>170</v>
@@ -4678,7 +4699,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>173</v>
       </c>

</xml_diff>